<commit_message>
Switched California rates from E20 to B20
</commit_message>
<xml_diff>
--- a/WWTP_Billing_Assumptions.xlsx
+++ b/WWTP_Billing_Assumptions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="166925"/>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{9292D116-ACE5-4853-9778-C619E8177B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -323,39 +323,56 @@
   <si>
     <t>Ignore gas if no CHP</t>
   </si>
+  <si>
+    <t>Industrial Rate w/ Generation: B-20 at Primary Voltage</t>
+  </si>
+  <si>
+    <t>Industrial Rate: E-20 at Primary Voltage</t>
+  </si>
+  <si>
+    <t>Industrial Rate B-20 at Primary Voltage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -368,15 +385,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -699,17 +726,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="A36" workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
     <col min="2" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -772,7 +798,7 @@
         <v>12000053001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30">
+    <row ht="30" r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -780,7 +806,7 @@
         <v>48003033002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30">
+    <row ht="30" r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -802,9 +828,9 @@
         <v>36001010006</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30">
+    <row ht="30" r="6" spans="1:15">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -867,7 +893,7 @@
         <v>6004009001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30">
+    <row ht="30" r="9" spans="1:15">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -908,7 +934,7 @@
         <v>36002001011</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -927,7 +953,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="11" spans="1:15">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -950,7 +976,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="12" spans="1:15">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -969,7 +995,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="13" spans="1:15">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -988,7 +1014,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="14" spans="1:15">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1015,7 +1041,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="15" spans="1:15">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1040,7 +1066,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="16" spans="1:15">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1061,7 +1087,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1080,7 +1106,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="18" spans="1:13">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1099,7 +1125,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="19" spans="1:13">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1118,7 +1144,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="20" spans="1:13">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1137,7 +1163,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1158,7 +1184,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="22" spans="1:13">
       <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
@@ -1181,7 +1207,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="23" spans="1:13">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1206,7 +1232,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="24" spans="1:13">
       <c r="A24" s="3" t="s">
         <v>37</v>
       </c>
@@ -1225,7 +1251,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
@@ -1244,7 +1270,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="26" spans="1:13">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1263,7 +1289,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
@@ -1282,7 +1308,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
@@ -1301,7 +1327,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
@@ -1322,7 +1348,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -1341,7 +1367,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
@@ -1360,7 +1386,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>45</v>
       </c>
@@ -1379,7 +1405,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="33" spans="1:15">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -1398,7 +1424,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="34" spans="1:15">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
@@ -1436,7 +1462,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="30">
+    <row ht="30" r="36" spans="1:15">
       <c r="A36" s="3" t="s">
         <v>49</v>
       </c>
@@ -1467,7 +1493,7 @@
         <v>17000721001</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="38" spans="1:15">
       <c r="A38" s="3" t="s">
         <v>51</v>
       </c>
@@ -1525,7 +1551,7 @@
         <v>6009031001</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="30">
+    <row ht="30" r="40" spans="1:15">
       <c r="A40" s="3" t="s">
         <v>53</v>
       </c>
@@ -1566,7 +1592,7 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="30">
+    <row ht="30" r="41" spans="1:15">
       <c r="A41" s="3" t="s">
         <v>54</v>
       </c>
@@ -1592,7 +1618,7 @@
         <v>34002065001</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="30">
+    <row ht="30" r="42" spans="1:15">
       <c r="A42" s="3" t="s">
         <v>55</v>
       </c>
@@ -1618,7 +1644,7 @@
         <v>47001016001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="30">
+    <row ht="30" r="43" spans="1:15">
       <c r="A43" s="3" t="s">
         <v>56</v>
       </c>
@@ -1632,7 +1658,7 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="30">
+    <row ht="30" r="44" spans="1:15">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -1643,7 +1669,7 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30">
+    <row ht="30" r="45" spans="1:15">
       <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
@@ -1651,7 +1677,7 @@
         <v>39002093001</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30">
+    <row ht="30" r="46" spans="1:15">
       <c r="A46" s="3" t="s">
         <v>59</v>
       </c>
@@ -1659,7 +1685,7 @@
         <v>10000027001</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="30">
+    <row ht="30" r="47" spans="1:15">
       <c r="A47" s="3" t="s">
         <v>60</v>
       </c>
@@ -1670,7 +1696,7 @@
         <v>13000012004</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="30">
+    <row ht="30" r="48" spans="1:15">
       <c r="A48" s="3" t="s">
         <v>61</v>
       </c>
@@ -1681,7 +1707,7 @@
         <v>29001011001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="45">
+    <row ht="45" r="49" spans="1:2">
       <c r="A49" s="3" t="s">
         <v>62</v>
       </c>
@@ -1696,14 +1722,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85995C10-2ADA-4E06-99AB-80C6038BFB63}">
-  <dimension ref="A1:M51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85995C10-2ADA-4E06-99AB-80C6038BFB63}">
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection pane="topLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -1775,7 +1800,7 @@
         <v>8000070001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30">
+    <row ht="30" r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>66</v>
       </c>
@@ -1798,7 +1823,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="30">
+    <row ht="30" r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>68</v>
       </c>
@@ -1811,7 +1836,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="30">
+    <row ht="30" r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
@@ -1841,7 +1866,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="30">
+    <row ht="30" r="10" spans="1:13">
       <c r="A10" s="3" t="s">
         <v>71</v>
       </c>
@@ -1941,7 +1966,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="30">
+    <row ht="30" r="15" spans="1:13">
       <c r="A15" s="3" t="s">
         <v>75</v>
       </c>
@@ -1963,7 +1988,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="16" spans="1:13">
       <c r="A16" s="3" t="s">
         <v>76</v>
       </c>
@@ -2008,7 +2033,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="19" spans="1:13">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -2027,7 +2052,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="20" spans="1:13">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2046,7 +2071,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="21" spans="1:13">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2065,7 +2090,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="22" spans="1:13">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2084,7 +2109,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="23" spans="1:13">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -2105,7 +2130,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="24" spans="1:13">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2130,7 +2155,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2174,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="26" spans="1:13">
       <c r="A26" s="3" t="s">
         <v>86</v>
       </c>
@@ -2168,7 +2193,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>87</v>
       </c>
@@ -2187,7 +2212,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>88</v>
       </c>
@@ -2206,7 +2231,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>89</v>
       </c>
@@ -2225,7 +2250,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>90</v>
       </c>
@@ -2244,7 +2269,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>91</v>
       </c>
@@ -2263,7 +2288,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>92</v>
       </c>
@@ -2282,7 +2307,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>93</v>
       </c>
@@ -2301,7 +2326,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
@@ -2320,7 +2345,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>96</v>
       </c>
@@ -2339,7 +2364,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="36" spans="1:13">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -2358,7 +2383,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" ht="30" customHeight="1">
+    <row ht="30" customHeight="1" r="37" spans="1:13">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2373,7 +2398,7 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="38" spans="1:13">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2388,7 +2413,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="39" spans="1:13">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2403,7 +2428,7 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="40" spans="1:13">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2418,7 +2443,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="41" spans="1:13">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2433,7 +2458,7 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="42" spans="1:13">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2448,7 +2473,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="43" spans="1:13">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2463,7 +2488,7 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13" ht="15" customHeight="1">
+    <row ht="15" customHeight="1" r="44" spans="1:13">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>

</xml_diff>